<commit_message>
remake logic and pages with orders
</commit_message>
<xml_diff>
--- a/WebApplication14/wwwroot/1e70d8b4-de18-48ea-8700-5bf3117e7328.xlsx
+++ b/WebApplication14/wwwroot/1e70d8b4-de18-48ea-8700-5bf3117e7328.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -36,6 +36,15 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Vase</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
   </si>
 </sst>
 </file>
@@ -81,7 +90,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -118,7 +127,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0">
         <v>24</v>
@@ -128,8 +137,28 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0">
+        <v>5</v>
+      </c>
+      <c r="E3" s="0">
+        <v>120</v>
+      </c>
       <c r="F3" s="0">
-        <v>144</v>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" s="0">
+        <v>744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add  adaptive and responsive design to webpages.
</commit_message>
<xml_diff>
--- a/WebApplication14/wwwroot/1e70d8b4-de18-48ea-8700-5bf3117e7328.xlsx
+++ b/WebApplication14/wwwroot/1e70d8b4-de18-48ea-8700-5bf3117e7328.xlsx
@@ -127,7 +127,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E2" s="0">
         <v>24</v>
@@ -147,7 +147,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="0">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="0">
         <v>120</v>

</xml_diff>

<commit_message>
Remake some paypal payments orders
</commit_message>
<xml_diff>
--- a/WebApplication14/wwwroot/1e70d8b4-de18-48ea-8700-5bf3117e7328.xlsx
+++ b/WebApplication14/wwwroot/1e70d8b4-de18-48ea-8700-5bf3117e7328.xlsx
@@ -32,13 +32,13 @@
     <t>TotalCost</t>
   </si>
   <si>
-    <t>выфвыф</t>
+    <t>Vase</t>
   </si>
   <si>
-    <t>ывыфвфыв</t>
+    <t>Cat</t>
   </si>
   <si>
-    <t>USA</t>
+    <t>Ukraine</t>
   </si>
 </sst>
 </file>
@@ -121,18 +121,18 @@
         <v>8</v>
       </c>
       <c r="D2" s="0">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E2" s="0">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="F2" s="0">
-        <v>24</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3">
       <c r="F3" s="0">
-        <v>24</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>